<commit_message>
Update outdated URL on About tab
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="24915" windowHeight="11580"/>
+    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,9 +42,6 @@
     <t>U.S. Environmental Protection Agency</t>
   </si>
   <si>
-    <t>http://yosemite.epa.gov/EE%5Cepa%5Ceed.nsf/webpages/MortalityRiskValuation.html#whatvalue</t>
-  </si>
-  <si>
     <t>Frequently Asked Questions on Mortality Risk Valuation</t>
   </si>
   <si>
@@ -71,12 +79,15 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,6 +239,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -263,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,7 +483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -468,42 +513,42 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,12 +556,12 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -526,17 +571,20 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" location="whatvalue" display="https://www.epa.gov/environmental-economics/mortality-risk-valuation - whatvalue" xr:uid="{F4EA8DF9-36E3-4A47-8B4C-6E99399B200A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -554,15 +602,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f>7.4*10^6*About!A17</f>

</xml_diff>

<commit_message>
[add-outputs/VoaSL] update About sheet notes
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Desktop\Dropbox_Free_Zone\EPS\Model Repos\eps-us\InputData\add-outputs\VoaSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF28FF-AE75-49F4-8013-0ABB667283AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22200" yWindow="1920" windowWidth="21600" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>VoaSL Value of a Statistical Life</t>
   </si>
@@ -60,18 +60,6 @@
     <t>Statistical Life</t>
   </si>
   <si>
-    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
-  </si>
-  <si>
-    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
-  </si>
-  <si>
-    <t>here must reflect the one used to calculate the health impacts in that</t>
-  </si>
-  <si>
-    <t>variable for the result to be accurate.</t>
-  </si>
-  <si>
     <t>Currency Year Adjustment</t>
   </si>
   <si>
@@ -82,6 +70,12 @@
   </si>
   <si>
     <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
+  </si>
+  <si>
+    <t>This variable is used to convert estimated avoided premature mortalities</t>
+  </si>
+  <si>
+    <t>(calculated using data from HOIpTP) into a dollar amount.</t>
   </si>
 </sst>
 </file>
@@ -134,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -144,7 +138,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -164,9 +157,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,9 +197,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,26 +232,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,26 +267,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -484,9 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -518,7 +479,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,45 +493,32 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
+      <c r="A15">
+        <v>1.141</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -602,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
@@ -610,10 +558,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <f>7.4*10^6*About!A17</f>
+        <f>7.4*10^6*About!A15</f>
         <v>8443400</v>
       </c>
     </row>

</xml_diff>